<commit_message>
Ora riconosce 31 foto. Sistemati commenti e ordine
</commit_message>
<xml_diff>
--- a/Confronto risultati.xlsx
+++ b/Confronto risultati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabiola\Desktop\Progetto ESI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3072DC91-3A04-4C35-9E98-1448850AD294}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DBF919-06E1-4A4F-890D-332E829306EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{09E0A96F-9B6D-4BE1-9B54-D1392097E3C4}"/>
   </bookViews>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:X49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1385,6 +1385,7 @@
     <col min="14" max="14" width="3.5546875" customWidth="1"/>
     <col min="16" max="16" width="10.6640625" customWidth="1"/>
     <col min="17" max="17" width="2.33203125" customWidth="1"/>
+    <col min="21" max="21" width="2.77734375" customWidth="1"/>
     <col min="23" max="23" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>